<commit_message>
sync: Export all json sorted by `RowOrder`
</commit_message>
<xml_diff>
--- a/export/v1.0.8/techtree.xlsx
+++ b/export/v1.0.8/techtree.xlsx
@@ -6,14 +6,16 @@
   </bookViews>
   <sheets>
     <sheet name="TechTree" sheetId="1" r:id="rId1"/>
-    <sheet name="ResearchRecipes" sheetId="2" r:id="rId3"/>
+    <sheet name="TechTree_Expanded" sheetId="2" r:id="rId3"/>
+    <sheet name="ResearchRecipes" sheetId="3" r:id="rId4"/>
+    <sheet name="Exploration_Order" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="514">
   <si>
     <t>CODE</t>
   </si>
@@ -66,7 +68,7 @@
     <t>Tier</t>
   </si>
   <si>
-    <t>Order</t>
+    <t>RowOrder</t>
   </si>
   <si>
     <t>BUILD_ANT_LAUNCHER</t>
@@ -1449,6 +1451,9 @@
     <t>IDEA_TOXICWASTE</t>
   </si>
   <si>
+    <t>TechTree with columns expanded as multiple rows</t>
+  </si>
+  <si>
     <t>CASTE</t>
   </si>
   <si>
@@ -1525,6 +1530,33 @@
   </si>
   <si>
     <t>RARE_FRUIT 50</t>
+  </si>
+  <si>
+    <t>ORDER</t>
+  </si>
+  <si>
+    <t>BiomeBlue2</t>
+  </si>
+  <si>
+    <t>BiomeBlue2_start</t>
+  </si>
+  <si>
+    <t>BiomeScrapara</t>
+  </si>
+  <si>
+    <t>BiomeGreen</t>
+  </si>
+  <si>
+    <t>BiomeBlue2, BiomeScrapara, BiomeGreen</t>
+  </si>
+  <si>
+    <t>BiomeToxicwaste</t>
+  </si>
+  <si>
+    <t>BiomeConcrete</t>
+  </si>
+  <si>
+    <t>BiomeBlue2, BiomeScrapara, BiomeGreen, BiomeToxicwaste, BiomeConcrete</t>
   </si>
 </sst>
 </file>
@@ -1532,9 +1564,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1558,13 +1594,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <d:dxf xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <font>
+        <color rgb="ff006400"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="ff90ee90"/>
+        </patternFill>
+      </fill>
+    </d:dxf>
+    <d:dxf xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <font>
+        <color rgb="ff006400"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="ff90ee90"/>
+        </patternFill>
+      </fill>
+    </d:dxf>
+    <d:dxf xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <font>
+        <color rgb="ff006400"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="ff90ee90"/>
+        </patternFill>
+      </fill>
+    </d:dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1589,7 +1657,7 @@
     <tableColumn id="15" name="AUTO DONE"/>
     <tableColumn id="16" name="Group"/>
     <tableColumn id="17" name="Tier"/>
-    <tableColumn id="18" name="Order"/>
+    <tableColumn id="18" name="RowOrder"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1606,6 +1674,18 @@
     <tableColumn id="5" name="ENERGY"/>
     <tableColumn id="6" name="PRODUCT"/>
     <tableColumn id="7" name="PRODUCT QUANTITY"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Exploration_Order_Data" displayName="Exploration_Order_Data" ref="A1:C51" headerRowCount="1">
+  <autoFilter ref="A1:C51"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="ORDER"/>
+    <tableColumn id="2" name="BiomeBlue2"/>
+    <tableColumn id="3" name="RowOrder"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1636,7 +1716,7 @@
     <col min="15" max="15" width="14.46933650970459" customWidth="1"/>
     <col min="16" max="16" width="11.442831039428711" customWidth="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.655442237854004" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7667,6 +7747,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:R240">
+    <cfRule priority="1" type="cellIs" operator="equal" dxfId="0">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <headerFooter/>
   <tableParts>
     <tablePart r:id="rId1"/>
@@ -7675,6 +7760,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule priority="1" type="cellIs" operator="equal" dxfId="0">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -7699,36 +7807,36 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E2" s="0">
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G2" s="0">
         <v>10</v>
@@ -7736,16 +7844,16 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E3" s="0">
         <v>50</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G3" s="0">
         <v>10</v>
@@ -7753,16 +7861,16 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E4" s="0">
         <v>250</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G4" s="0">
         <v>10</v>
@@ -7770,16 +7878,16 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G5" s="0">
         <v>5</v>
@@ -7787,16 +7895,16 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>493</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>494</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>492</v>
       </c>
       <c r="G6" s="0">
         <v>25</v>
@@ -7804,16 +7912,16 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="G7" s="0">
         <v>60</v>
@@ -7821,16 +7929,16 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G8" s="0">
         <v>5</v>
@@ -7838,16 +7946,16 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>500</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>501</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>499</v>
       </c>
       <c r="G9" s="0">
         <v>25</v>
@@ -7855,19 +7963,606 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G10" s="0">
         <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G10">
+    <cfRule priority="1" type="cellIs" operator="equal" dxfId="0">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <headerFooter/>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.816435813903809" customWidth="1"/>
+    <col min="2" max="2" width="69.25420379638672" customWidth="1"/>
+    <col min="3" max="3" width="12.655442237854004" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C2" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C4" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="C5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C6" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="C7" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C8" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C9" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>8</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C10" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>9</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C11" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>10</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C12" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>11</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C13" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C14" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C15" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C16" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>15</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C17" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>16</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C18" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>17</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C19" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>18</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C20" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C21" s="0">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>20</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C22" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>21</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C23" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>22</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C24" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>23</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C25" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>24</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C26" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>25</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C27" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>26</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C28" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>27</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C29" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>28</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C30" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>29</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C31" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>30</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C32" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>31</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C33" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C34" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>33</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C35" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>34</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C36" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>35</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C37" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>36</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C38" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>37</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C39" s="0">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>38</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C40" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C41" s="0">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>40</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C42" s="0">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>41</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C43" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>42</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C44" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>43</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C45" s="0">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>44</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C46" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>45</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C47" s="0">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>46</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C48" s="0">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>47</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C49" s="0">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>48</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C50" s="0">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>49</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C51" s="0">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exports: Added json for `loc`: tutorial, Instinct, techtree, credits, achievements
</commit_message>
<xml_diff>
--- a/export/v1.0.8/techtree.xlsx
+++ b/export/v1.0.8/techtree.xlsx
@@ -6,16 +6,15 @@
   </bookViews>
   <sheets>
     <sheet name="TechTree" sheetId="1" r:id="rId1"/>
-    <sheet name="TechTree_Expanded" sheetId="2" r:id="rId3"/>
-    <sheet name="ResearchRecipes" sheetId="3" r:id="rId4"/>
-    <sheet name="Exploration_Order" sheetId="4" r:id="rId5"/>
+    <sheet name="ResearchRecipes" sheetId="2" r:id="rId3"/>
+    <sheet name="Exploration_Order" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="513">
   <si>
     <t>CODE</t>
   </si>
@@ -1449,9 +1448,6 @@
   </si>
   <si>
     <t>IDEA_TOXICWASTE</t>
-  </si>
-  <si>
-    <t>TechTree with columns expanded as multiple rows</t>
   </si>
   <si>
     <t>CASTE</t>
@@ -1564,13 +1560,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="22"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -1594,24 +1586,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <d:dxf xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <font>
-        <color rgb="ff006400"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="ff90ee90"/>
-        </patternFill>
-      </fill>
-    </d:dxf>
+  <dxfs count="2">
     <d:dxf xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
       <font>
         <color rgb="ff006400"/>
@@ -7761,29 +7742,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>478</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A1">
-    <cfRule priority="1" type="cellIs" operator="equal" dxfId="0">
-      <formula>"x"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7807,36 +7765,36 @@
         <v>2</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>479</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>480</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>481</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>482</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>484</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>485</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>486</v>
       </c>
       <c r="E2" s="0">
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G2" s="0">
         <v>10</v>
@@ -7844,16 +7802,16 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>487</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>488</v>
       </c>
       <c r="E3" s="0">
         <v>50</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G3" s="0">
         <v>10</v>
@@ -7861,16 +7819,16 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>489</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>490</v>
       </c>
       <c r="E4" s="0">
         <v>250</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G4" s="0">
         <v>10</v>
@@ -7878,16 +7836,16 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>491</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>492</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>493</v>
       </c>
       <c r="G5" s="0">
         <v>5</v>
@@ -7895,16 +7853,16 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>494</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>495</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G6" s="0">
         <v>25</v>
@@ -7912,16 +7870,16 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>496</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>497</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G7" s="0">
         <v>60</v>
@@ -7929,16 +7887,16 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>498</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>499</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>500</v>
       </c>
       <c r="G8" s="0">
         <v>5</v>
@@ -7946,16 +7904,16 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>501</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>502</v>
-      </c>
       <c r="F9" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G9" s="0">
         <v>25</v>
@@ -7963,16 +7921,16 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>503</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>490</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>504</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G10" s="0">
         <v>60</v>
@@ -7991,7 +7949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C51"/>
   <sheetViews>
@@ -8006,10 +7964,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>505</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>506</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>17</v>
@@ -8020,7 +7978,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
@@ -8031,7 +7989,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C3" s="0">
         <v>1</v>
@@ -8042,7 +8000,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C4" s="0">
         <v>2</v>
@@ -8053,7 +8011,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C5" s="0">
         <v>3</v>
@@ -8064,7 +8022,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C6" s="0">
         <v>4</v>
@@ -8075,7 +8033,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C7" s="0">
         <v>5</v>
@@ -8086,7 +8044,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C8" s="0">
         <v>6</v>
@@ -8097,7 +8055,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C9" s="0">
         <v>7</v>
@@ -8108,7 +8066,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C10" s="0">
         <v>8</v>
@@ -8119,7 +8077,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C11" s="0">
         <v>9</v>
@@ -8130,7 +8088,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C12" s="0">
         <v>10</v>
@@ -8141,7 +8099,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C13" s="0">
         <v>11</v>
@@ -8152,7 +8110,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C14" s="0">
         <v>12</v>
@@ -8163,7 +8121,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C15" s="0">
         <v>13</v>
@@ -8174,7 +8132,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C16" s="0">
         <v>14</v>
@@ -8185,7 +8143,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C17" s="0">
         <v>15</v>
@@ -8196,7 +8154,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C18" s="0">
         <v>16</v>
@@ -8207,7 +8165,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C19" s="0">
         <v>17</v>
@@ -8218,7 +8176,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C20" s="0">
         <v>18</v>
@@ -8229,7 +8187,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C21" s="0">
         <v>19</v>
@@ -8240,7 +8198,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C22" s="0">
         <v>20</v>
@@ -8251,7 +8209,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C23" s="0">
         <v>21</v>
@@ -8262,7 +8220,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C24" s="0">
         <v>22</v>
@@ -8273,7 +8231,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C25" s="0">
         <v>23</v>
@@ -8284,7 +8242,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C26" s="0">
         <v>24</v>
@@ -8295,7 +8253,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C27" s="0">
         <v>25</v>
@@ -8306,7 +8264,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C28" s="0">
         <v>26</v>
@@ -8317,7 +8275,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C29" s="0">
         <v>27</v>
@@ -8328,7 +8286,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C30" s="0">
         <v>28</v>
@@ -8339,7 +8297,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C31" s="0">
         <v>29</v>
@@ -8350,7 +8308,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C32" s="0">
         <v>30</v>
@@ -8361,7 +8319,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C33" s="0">
         <v>31</v>
@@ -8372,7 +8330,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C34" s="0">
         <v>32</v>
@@ -8383,7 +8341,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C35" s="0">
         <v>33</v>
@@ -8394,7 +8352,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C36" s="0">
         <v>34</v>
@@ -8405,7 +8363,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C37" s="0">
         <v>35</v>
@@ -8416,7 +8374,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C38" s="0">
         <v>36</v>
@@ -8427,7 +8385,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C39" s="0">
         <v>37</v>
@@ -8438,7 +8396,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C40" s="0">
         <v>38</v>
@@ -8449,7 +8407,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C41" s="0">
         <v>39</v>
@@ -8460,7 +8418,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C42" s="0">
         <v>40</v>
@@ -8471,7 +8429,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C43" s="0">
         <v>41</v>
@@ -8482,7 +8440,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C44" s="0">
         <v>42</v>
@@ -8493,7 +8451,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C45" s="0">
         <v>43</v>
@@ -8504,7 +8462,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C46" s="0">
         <v>44</v>
@@ -8515,7 +8473,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C47" s="0">
         <v>45</v>
@@ -8526,7 +8484,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C48" s="0">
         <v>46</v>
@@ -8537,7 +8495,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C49" s="0">
         <v>47</v>
@@ -8548,7 +8506,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C50" s="0">
         <v>48</v>
@@ -8559,7 +8517,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C51" s="0">
         <v>49</v>

</xml_diff>